<commit_message>
dryweights data input is ongoing
</commit_message>
<xml_diff>
--- a/dryweights.xlsx
+++ b/dryweights.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="333">
   <si>
     <t xml:space="preserve">Genotype</t>
   </si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t xml:space="preserve">1479+LN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">2416+HN</t>
@@ -1113,10 +1116,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G326"/>
+  <dimension ref="A1:O326"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O244" activeCellId="0" sqref="O244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1178,6 +1181,21 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>6.13</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>327.7</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>147.8</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>202.2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>229.8</v>
+      </c>
       <c r="G5" s="0" t="n">
         <v>1.67</v>
       </c>
@@ -1186,6 +1204,21 @@
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>342.9</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>386.5</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>407.8</v>
+      </c>
       <c r="G6" s="0" t="n">
         <v>2.1</v>
       </c>
@@ -1194,6 +1227,21 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>12.31</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>447.2</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>380.8</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>274.7</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>481.9</v>
+      </c>
       <c r="G7" s="0" t="n">
         <v>3.79</v>
       </c>
@@ -1368,6 +1416,21 @@
       <c r="A25" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>287.8</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>385.7</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>366</v>
+      </c>
       <c r="G25" s="0" t="n">
         <v>1.98</v>
       </c>
@@ -1462,6 +1525,21 @@
       <c r="A33" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <v>6.66</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>330.11</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>370.1</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>345.1</v>
+      </c>
       <c r="G33" s="0" t="n">
         <v>1.68</v>
       </c>
@@ -1470,6 +1548,21 @@
       <c r="A34" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <v>9.71</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>394.3</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>329.2</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>341.8</v>
+      </c>
       <c r="G34" s="0" t="n">
         <v>2.1</v>
       </c>
@@ -1478,6 +1571,21 @@
       <c r="A35" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="B35" s="0" t="n">
+        <v>6.96</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>312.5</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>303.1</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>315.2</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>376.1</v>
+      </c>
       <c r="G35" s="0" t="n">
         <v>1.87</v>
       </c>
@@ -1586,6 +1694,21 @@
       <c r="A41" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="B41" s="0" t="n">
+        <v>12.03</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>534.1</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>371.8</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>413.6</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>454.3</v>
+      </c>
       <c r="G41" s="0" t="n">
         <v>3.31</v>
       </c>
@@ -1594,6 +1717,21 @@
       <c r="A42" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="B42" s="0" t="n">
+        <v>13.96</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>572.7</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>384.9</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>425.9</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>372.6</v>
+      </c>
       <c r="G42" s="0" t="n">
         <v>3.55</v>
       </c>
@@ -1602,6 +1740,21 @@
       <c r="A43" s="0" t="s">
         <v>48</v>
       </c>
+      <c r="B43" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>512.8</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>391.8</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>496</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>538.9</v>
+      </c>
       <c r="G43" s="0" t="n">
         <v>3.1</v>
       </c>
@@ -1784,6 +1937,21 @@
       <c r="A62" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="B62" s="0" t="n">
+        <v>8.18</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>345.25</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>410.7</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>417.2</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>456.3</v>
+      </c>
       <c r="G62" s="0" t="n">
         <v>1.88</v>
       </c>
@@ -1904,6 +2072,21 @@
       <c r="A77" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="B77" s="0" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>508.5</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>352.7</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>387.4</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>394.8</v>
+      </c>
       <c r="G77" s="0" t="n">
         <v>2.91</v>
       </c>
@@ -1920,6 +2103,21 @@
       <c r="A79" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="B79" s="0" t="n">
+        <v>9.89</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>401.1</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>294.4</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>448.6</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>425.9</v>
+      </c>
       <c r="G79" s="0" t="n">
         <v>2.61</v>
       </c>
@@ -1944,6 +2142,21 @@
       <c r="A82" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="B82" s="0" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>416.9</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>364.4</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>407.1</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>416.5</v>
+      </c>
       <c r="G82" s="0" t="n">
         <v>2.45</v>
       </c>
@@ -1952,6 +2165,21 @@
       <c r="A83" s="0" t="s">
         <v>88</v>
       </c>
+      <c r="B83" s="0" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>519</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>427.5</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>613.6</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>502.2</v>
+      </c>
       <c r="G83" s="0" t="n">
         <v>3.76</v>
       </c>
@@ -1960,6 +2188,21 @@
       <c r="A84" s="0" t="s">
         <v>89</v>
       </c>
+      <c r="B84" s="0" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>408</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>168.4</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>254.7</v>
+      </c>
       <c r="G84" s="0" t="n">
         <v>2.38</v>
       </c>
@@ -1968,6 +2211,21 @@
       <c r="A85" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="B85" s="0" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>367.8</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>287.8</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>383.2</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>462.2</v>
+      </c>
       <c r="G85" s="0" t="n">
         <v>2.21</v>
       </c>
@@ -1976,6 +2234,21 @@
       <c r="A86" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="B86" s="0" t="n">
+        <v>7.53</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>389</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>237.7</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>258.3</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>306.4</v>
+      </c>
       <c r="G86" s="0" t="n">
         <v>2.09</v>
       </c>
@@ -1984,6 +2257,21 @@
       <c r="A87" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="B87" s="0" t="n">
+        <v>6.71</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>313</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>228.5</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>260.5</v>
+      </c>
       <c r="G87" s="0" t="n">
         <v>1.74</v>
       </c>
@@ -2064,6 +2352,21 @@
       <c r="A97" s="0" t="s">
         <v>102</v>
       </c>
+      <c r="B97" s="0" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>262.7</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>305.3</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>450.1</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>437.9</v>
+      </c>
       <c r="G97" s="0" t="n">
         <v>1.49</v>
       </c>
@@ -2072,6 +2375,21 @@
       <c r="A98" s="0" t="s">
         <v>103</v>
       </c>
+      <c r="B98" s="0" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>410</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>389.6</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>442.1</v>
+      </c>
       <c r="G98" s="0" t="n">
         <v>2.18</v>
       </c>
@@ -2096,6 +2414,21 @@
       <c r="A101" s="0" t="s">
         <v>106</v>
       </c>
+      <c r="B101" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>507.5</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>273.6</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>339.5</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>357.3</v>
+      </c>
       <c r="G101" s="0" t="n">
         <v>2.84</v>
       </c>
@@ -2127,6 +2460,21 @@
       <c r="A103" s="0" t="s">
         <v>108</v>
       </c>
+      <c r="B103" s="0" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>593.3</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>331.1</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>383.2</v>
+      </c>
       <c r="G103" s="0" t="n">
         <v>3.57</v>
       </c>
@@ -2158,6 +2506,21 @@
       <c r="A105" s="0" t="s">
         <v>110</v>
       </c>
+      <c r="B105" s="0" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>253.9</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>314.1</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>297.3</v>
+      </c>
       <c r="G105" s="0" t="n">
         <v>1.36</v>
       </c>
@@ -2182,6 +2545,21 @@
       <c r="A108" s="0" t="s">
         <v>113</v>
       </c>
+      <c r="B108" s="0" t="n">
+        <v>11.04</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>443.6</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>435.9</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>494.8</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>500.3</v>
+      </c>
       <c r="G108" s="0" t="n">
         <v>2.81</v>
       </c>
@@ -2198,6 +2576,21 @@
       <c r="A110" s="0" t="s">
         <v>115</v>
       </c>
+      <c r="B110" s="0" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>397.7</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>387.4</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>472</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>485.9</v>
+      </c>
       <c r="G110" s="0" t="n">
         <v>2.69</v>
       </c>
@@ -2214,6 +2607,12 @@
       <c r="A112" s="0" t="s">
         <v>117</v>
       </c>
+      <c r="B112" s="0" t="n">
+        <v>15.83</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>610</v>
+      </c>
       <c r="G112" s="0" t="n">
         <v>4.13</v>
       </c>
@@ -2222,6 +2621,12 @@
       <c r="A113" s="0" t="s">
         <v>118</v>
       </c>
+      <c r="B113" s="0" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>621</v>
+      </c>
       <c r="G113" s="0" t="n">
         <v>3.74</v>
       </c>
@@ -2333,6 +2738,21 @@
       <c r="A125" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="B125" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>398.9</v>
+      </c>
+      <c r="D125" s="0" t="n">
+        <v>469.4</v>
+      </c>
+      <c r="E125" s="0" t="n">
+        <v>508.5</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>541.1</v>
+      </c>
       <c r="G125" s="0" t="n">
         <v>3</v>
       </c>
@@ -2395,6 +2815,21 @@
       <c r="A129" s="0" t="s">
         <v>134</v>
       </c>
+      <c r="B129" s="0" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>340.6</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>303.1</v>
+      </c>
+      <c r="E129" s="0" t="n">
+        <v>454.3</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>470.7</v>
+      </c>
       <c r="G129" s="0" t="n">
         <v>2.38</v>
       </c>
@@ -2403,6 +2838,21 @@
       <c r="A130" s="0" t="s">
         <v>135</v>
       </c>
+      <c r="B130" s="0" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>246.4</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>195.3</v>
+      </c>
+      <c r="E130" s="0" t="n">
+        <v>284.5</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>364.4</v>
+      </c>
       <c r="G130" s="0" t="n">
         <v>1.36</v>
       </c>
@@ -2512,6 +2962,21 @@
       <c r="A138" s="0" t="s">
         <v>143</v>
       </c>
+      <c r="B138" s="0" t="n">
+        <v>8.38</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>407.1</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>442.1</v>
+      </c>
       <c r="G138" s="0" t="n">
         <v>2.14</v>
       </c>
@@ -2520,6 +2985,21 @@
       <c r="A139" s="0" t="s">
         <v>144</v>
       </c>
+      <c r="B139" s="0" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>389.6</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>273.6</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>205.2</v>
+      </c>
       <c r="G139" s="0" t="n">
         <v>1.8</v>
       </c>
@@ -2669,6 +3149,21 @@
       <c r="A152" s="0" t="s">
         <v>157</v>
       </c>
+      <c r="B152" s="0" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>347.55</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>583.2</v>
+      </c>
+      <c r="E152" s="0" t="n">
+        <v>456.3</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>448.6</v>
+      </c>
       <c r="G152" s="0" t="n">
         <v>2.13</v>
       </c>
@@ -2849,6 +3344,21 @@
       <c r="A167" s="0" t="s">
         <v>172</v>
       </c>
+      <c r="B167" s="0" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>352.4</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>304.2</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>397.2</v>
+      </c>
       <c r="G167" s="0" t="n">
         <v>1.96</v>
       </c>
@@ -2857,6 +3367,21 @@
       <c r="A168" s="0" t="s">
         <v>173</v>
       </c>
+      <c r="B168" s="0" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>387</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>317.9</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>333.9</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>274.7</v>
+      </c>
       <c r="G168" s="0" t="n">
         <v>2.47</v>
       </c>
@@ -2929,6 +3454,21 @@
       <c r="A177" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="B177" s="0" t="n">
+        <v>6.89</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>305.3</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>324.5</v>
+      </c>
       <c r="G177" s="0" t="n">
         <v>1.97</v>
       </c>
@@ -2945,6 +3485,21 @@
       <c r="A179" s="0" t="s">
         <v>184</v>
       </c>
+      <c r="B179" s="0" t="n">
+        <v>12.19</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>394.8</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>509.1</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>543.2</v>
+      </c>
       <c r="G179" s="0" t="n">
         <v>3.45</v>
       </c>
@@ -2953,6 +3508,21 @@
       <c r="A180" s="0" t="s">
         <v>185</v>
       </c>
+      <c r="B180" s="0" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>289</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>273.6</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>141.3</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>401.3</v>
+      </c>
       <c r="G180" s="0" t="n">
         <v>1.16</v>
       </c>
@@ -2961,6 +3531,21 @@
       <c r="A181" s="0" t="s">
         <v>186</v>
       </c>
+      <c r="B181" s="0" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>252.8</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>254.7</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>259.4</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>349.8</v>
+      </c>
       <c r="G181" s="0" t="n">
         <v>1.24</v>
       </c>
@@ -2969,6 +3554,21 @@
       <c r="A182" s="0" t="s">
         <v>187</v>
       </c>
+      <c r="B182" s="0" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>304</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>258.3</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>339.5</v>
+      </c>
       <c r="G182" s="0" t="n">
         <v>1.55</v>
       </c>
@@ -2985,6 +3585,21 @@
       <c r="A184" s="0" t="s">
         <v>189</v>
       </c>
+      <c r="B184" s="0" t="n">
+        <v>10.57</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>211.7</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>266.6</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>376.1</v>
+      </c>
       <c r="G184" s="0" t="n">
         <v>2.68</v>
       </c>
@@ -3017,6 +3632,21 @@
       <c r="A188" s="0" t="s">
         <v>193</v>
       </c>
+      <c r="B188" s="0" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>519.6</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>356.4</v>
+      </c>
+      <c r="E188" s="0" t="n">
+        <v>407.1</v>
+      </c>
+      <c r="F188" s="0" t="n">
+        <v>525.2</v>
+      </c>
       <c r="G188" s="0" t="n">
         <v>3.31</v>
       </c>
@@ -3025,6 +3655,21 @@
       <c r="A189" s="0" t="s">
         <v>194</v>
       </c>
+      <c r="B189" s="0" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>468.8</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>322.6</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>376.1</v>
+      </c>
+      <c r="F189" s="0" t="n">
+        <v>424.3</v>
+      </c>
       <c r="G189" s="0" t="n">
         <v>2.69</v>
       </c>
@@ -3041,6 +3686,21 @@
       <c r="A191" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="B191" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C191" s="0" t="n">
+        <v>290.2</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>166.4</v>
+      </c>
+      <c r="E191" s="0" t="n">
+        <v>231.1</v>
+      </c>
+      <c r="F191" s="0" t="n">
+        <v>308.6</v>
+      </c>
       <c r="G191" s="0" t="n">
         <v>1.43</v>
       </c>
@@ -3065,6 +3725,21 @@
       <c r="A194" s="0" t="s">
         <v>199</v>
       </c>
+      <c r="B194" s="0" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <v>403.9</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>291.1</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>350.8</v>
+      </c>
+      <c r="F194" s="0" t="n">
+        <v>408.5</v>
+      </c>
       <c r="G194" s="0" t="n">
         <v>2.25</v>
       </c>
@@ -3132,10 +3807,13 @@
       <c r="G202" s="0" t="n">
         <v>3.17</v>
       </c>
+      <c r="O202" s="0" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G203" s="0" t="n">
         <v>1.94</v>
@@ -3143,7 +3821,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G204" s="0" t="n">
         <v>2.25</v>
@@ -3151,7 +3829,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>7.48</v>
@@ -3174,7 +3852,22 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>9.31</v>
+      </c>
+      <c r="C206" s="0" t="n">
+        <v>369</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>344.2</v>
+      </c>
+      <c r="E206" s="0" t="n">
+        <v>415</v>
+      </c>
+      <c r="F206" s="0" t="n">
+        <v>386.5</v>
       </c>
       <c r="G206" s="0" t="n">
         <v>2.31</v>
@@ -3182,7 +3875,22 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="C207" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="D207" s="0" t="n">
+        <v>202.2</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>306.4</v>
+      </c>
+      <c r="F207" s="0" t="n">
+        <v>389.6</v>
       </c>
       <c r="G207" s="0" t="n">
         <v>2.62</v>
@@ -3190,7 +3898,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G208" s="0" t="n">
         <v>2.3</v>
@@ -3198,7 +3906,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G209" s="0" t="n">
         <v>3.82</v>
@@ -3206,7 +3914,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G210" s="0" t="n">
         <v>4.1</v>
@@ -3214,7 +3922,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G211" s="0" t="n">
         <v>2.04</v>
@@ -3222,7 +3930,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G212" s="0" t="n">
         <v>2.5</v>
@@ -3230,7 +3938,22 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C213" s="0" t="n">
+        <v>490</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>336.7</v>
+      </c>
+      <c r="E213" s="0" t="n">
+        <v>397.2</v>
+      </c>
+      <c r="F213" s="0" t="n">
+        <v>414.3</v>
       </c>
       <c r="G213" s="0" t="n">
         <v>2.81</v>
@@ -3238,7 +3961,13 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="C214" s="0" t="n">
+        <v>562</v>
       </c>
       <c r="G214" s="0" t="n">
         <v>3.32</v>
@@ -3246,7 +3975,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G215" s="0" t="n">
         <v>2.52</v>
@@ -3254,7 +3983,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G216" s="0" t="n">
         <v>2.91</v>
@@ -3262,7 +3991,22 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>7.64</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="D217" s="0" t="n">
+        <v>195.3</v>
+      </c>
+      <c r="E217" s="0" t="n">
+        <v>267.9</v>
+      </c>
+      <c r="F217" s="0" t="n">
+        <v>319.8</v>
       </c>
       <c r="G217" s="0" t="n">
         <v>2</v>
@@ -3270,7 +4014,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G218" s="0" t="n">
         <v>1.99</v>
@@ -3278,7 +4022,22 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="C219" s="0" t="n">
+        <v>272.9</v>
+      </c>
+      <c r="D219" s="0" t="n">
+        <v>371.8</v>
+      </c>
+      <c r="E219" s="0" t="n">
+        <v>412.1</v>
+      </c>
+      <c r="F219" s="0" t="n">
+        <v>400.5</v>
       </c>
       <c r="G219" s="0" t="n">
         <v>1.48</v>
@@ -3286,7 +4045,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G220" s="0" t="n">
         <v>1.49</v>
@@ -3294,7 +4053,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G221" s="0" t="n">
         <v>1.8</v>
@@ -3302,7 +4061,22 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>5.45</v>
+      </c>
+      <c r="C222" s="0" t="n">
+        <v>255.8</v>
+      </c>
+      <c r="D222" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="E222" s="0" t="n">
+        <v>333.9</v>
+      </c>
+      <c r="F222" s="0" t="n">
+        <v>404.6</v>
       </c>
       <c r="G222" s="0" t="n">
         <v>1.22</v>
@@ -3310,7 +4084,22 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="B223" s="0" t="n">
+        <v>8.38</v>
+      </c>
+      <c r="C223" s="0" t="n">
+        <v>398.5</v>
+      </c>
+      <c r="D223" s="0" t="n">
+        <v>225.9</v>
+      </c>
+      <c r="E223" s="0" t="n">
+        <v>286.4</v>
+      </c>
+      <c r="F223" s="0" t="n">
+        <v>328.3</v>
       </c>
       <c r="G223" s="0" t="n">
         <v>2.08</v>
@@ -3318,7 +4107,22 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>7.99</v>
+      </c>
+      <c r="C224" s="0" t="n">
+        <v>397</v>
+      </c>
+      <c r="D224" s="0" t="n">
+        <v>227.2</v>
+      </c>
+      <c r="E224" s="0" t="n">
+        <v>305.3</v>
+      </c>
+      <c r="F224" s="0" t="n">
+        <v>326.4</v>
       </c>
       <c r="G224" s="0" t="n">
         <v>1.93</v>
@@ -3326,7 +4130,22 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>11.99</v>
+      </c>
+      <c r="C225" s="0" t="n">
+        <v>486</v>
+      </c>
+      <c r="D225" s="0" t="n">
+        <v>294.4</v>
+      </c>
+      <c r="E225" s="0" t="n">
+        <v>332</v>
+      </c>
+      <c r="F225" s="0" t="n">
+        <v>425.1</v>
       </c>
       <c r="G225" s="0" t="n">
         <v>2.99</v>
@@ -3334,7 +4153,22 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="B226" s="0" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="C226" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="D226" s="0" t="n">
+        <v>202.2</v>
+      </c>
+      <c r="E226" s="0" t="n">
+        <v>237.7</v>
+      </c>
+      <c r="F226" s="0" t="n">
+        <v>249.5</v>
       </c>
       <c r="G226" s="0" t="n">
         <v>2.22</v>
@@ -3342,7 +4176,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G227" s="0" t="n">
         <v>2.15</v>
@@ -3350,7 +4184,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G228" s="0" t="n">
         <v>3.76</v>
@@ -3358,7 +4192,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>9.1</v>
@@ -3381,7 +4215,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G230" s="0" t="n">
         <v>2.61</v>
@@ -3389,7 +4223,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>8.01</v>
@@ -3412,7 +4246,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G232" s="0" t="n">
         <v>3.46</v>
@@ -3420,7 +4254,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G233" s="0" t="n">
         <v>2.19</v>
@@ -3428,7 +4262,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G234" s="0" t="n">
         <v>1.9</v>
@@ -3436,7 +4270,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G235" s="0" t="n">
         <v>3.07</v>
@@ -3444,7 +4278,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G236" s="0" t="n">
         <v>3.62</v>
@@ -3452,7 +4286,22 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>9.69</v>
+      </c>
+      <c r="C237" s="0" t="n">
+        <v>436</v>
+      </c>
+      <c r="D237" s="0" t="n">
+        <v>392.5</v>
+      </c>
+      <c r="E237" s="0" t="n">
+        <v>315.2</v>
+      </c>
+      <c r="F237" s="0" t="n">
+        <v>262.7</v>
       </c>
       <c r="G237" s="0" t="n">
         <v>2.02</v>
@@ -3460,7 +4309,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>15.69</v>
@@ -3483,7 +4332,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G239" s="0" t="n">
         <v>2.06</v>
@@ -3491,7 +4340,22 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="C240" s="0" t="n">
+        <v>429</v>
+      </c>
+      <c r="D240" s="0" t="n">
+        <v>395.6</v>
+      </c>
+      <c r="E240" s="0" t="n">
+        <v>357.3</v>
+      </c>
+      <c r="F240" s="0" t="n">
+        <v>277.1</v>
       </c>
       <c r="G240" s="0" t="n">
         <v>2.37</v>
@@ -3499,7 +4363,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G241" s="0" t="n">
         <v>1.55</v>
@@ -3507,7 +4371,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G242" s="0" t="n">
         <v>2.98</v>
@@ -3515,7 +4379,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G243" s="0" t="n">
         <v>2.13</v>
@@ -3523,7 +4387,22 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="C244" s="0" t="n">
+        <v>402</v>
+      </c>
+      <c r="D244" s="0" t="n">
+        <v>361.9</v>
+      </c>
+      <c r="E244" s="0" t="n">
+        <v>384.1</v>
+      </c>
+      <c r="F244" s="0" t="n">
+        <v>307.5</v>
       </c>
       <c r="G244" s="0" t="n">
         <v>2.08</v>
@@ -3531,7 +4410,19 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="C245" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="D245" s="0" t="n">
+        <v>365.2</v>
+      </c>
+      <c r="E245" s="0" t="n">
+        <v>149.4</v>
       </c>
       <c r="G245" s="0" t="n">
         <v>1.21</v>
@@ -3539,7 +4430,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G246" s="0" t="n">
         <v>2.08</v>
@@ -3547,7 +4438,22 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>6.79</v>
+      </c>
+      <c r="C247" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="D247" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="E247" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="F247" s="0" t="n">
+        <v>198</v>
       </c>
       <c r="G247" s="0" t="n">
         <v>1.58</v>
@@ -3555,7 +4461,22 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>13.76</v>
+      </c>
+      <c r="C248" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="D248" s="0" t="n">
+        <v>442.8</v>
+      </c>
+      <c r="E248" s="0" t="n">
+        <v>433.3</v>
+      </c>
+      <c r="F248" s="0" t="n">
+        <v>437.9</v>
       </c>
       <c r="G248" s="0" t="n">
         <v>3.17</v>
@@ -3563,7 +4484,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G249" s="0" t="n">
         <v>2.98</v>
@@ -3571,7 +4492,22 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="C250" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="D250" s="0" t="n">
+        <v>428.9</v>
+      </c>
+      <c r="E250" s="0" t="n">
+        <v>375.2</v>
+      </c>
+      <c r="F250" s="0" t="n">
+        <v>296.4</v>
       </c>
       <c r="G250" s="0" t="n">
         <v>1.77</v>
@@ -3579,7 +4515,22 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>9.96</v>
+      </c>
+      <c r="C251" s="0" t="n">
+        <v>410</v>
+      </c>
+      <c r="D251" s="0" t="n">
+        <v>458.2</v>
+      </c>
+      <c r="E251" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="F251" s="0" t="n">
+        <v>378</v>
       </c>
       <c r="G251" s="0" t="n">
         <v>2.55</v>
@@ -3587,7 +4538,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G252" s="0" t="n">
         <v>2.43</v>
@@ -3595,7 +4546,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G253" s="0" t="n">
         <v>2.99</v>
@@ -3603,7 +4554,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G254" s="0" t="n">
         <v>2.34</v>
@@ -3611,7 +4562,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G255" s="0" t="n">
         <v>4.11</v>
@@ -3619,7 +4570,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G256" s="0" t="n">
         <v>4.74</v>
@@ -3627,7 +4578,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G257" s="0" t="n">
         <v>1.74</v>
@@ -3635,7 +4586,22 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="C258" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="D258" s="0" t="n">
+        <v>440.6</v>
+      </c>
+      <c r="E258" s="0" t="n">
+        <v>384.9</v>
+      </c>
+      <c r="F258" s="0" t="n">
+        <v>345.1</v>
       </c>
       <c r="G258" s="0" t="n">
         <v>2.01</v>
@@ -3643,7 +4609,22 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="C259" s="0" t="n">
+        <v>419</v>
+      </c>
+      <c r="D259" s="0" t="n">
+        <v>515.7</v>
+      </c>
+      <c r="E259" s="0" t="n">
+        <v>357.3</v>
+      </c>
+      <c r="F259" s="0" t="n">
+        <v>345.1</v>
       </c>
       <c r="G259" s="0" t="n">
         <v>2.25</v>
@@ -3651,7 +4632,22 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="C260" s="0" t="n">
+        <v>470</v>
+      </c>
+      <c r="D260" s="0" t="n">
+        <v>489.1</v>
+      </c>
+      <c r="E260" s="0" t="n">
+        <v>477.9</v>
+      </c>
+      <c r="F260" s="0" t="n">
+        <v>418</v>
       </c>
       <c r="G260" s="0" t="n">
         <v>3.34</v>
@@ -3659,7 +4655,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G261" s="0" t="n">
         <v>3.04</v>
@@ -3667,7 +4663,22 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="C262" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="D262" s="0" t="n">
+        <v>533.6</v>
+      </c>
+      <c r="E262" s="0" t="n">
+        <v>493.6</v>
+      </c>
+      <c r="F262" s="0" t="n">
+        <v>401.3</v>
       </c>
       <c r="G262" s="0" t="n">
         <v>2.64</v>
@@ -3675,7 +4686,22 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="C263" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="D263" s="0" t="n">
+        <v>317</v>
+      </c>
+      <c r="E263" s="0" t="n">
+        <v>385.7</v>
+      </c>
+      <c r="F263" s="0" t="n">
+        <v>415.8</v>
       </c>
       <c r="G263" s="0" t="n">
         <v>2.6</v>
@@ -3683,7 +4709,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>9.93</v>
@@ -3706,7 +4732,22 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>13.08</v>
+      </c>
+      <c r="C265" s="0" t="n">
+        <v>560</v>
+      </c>
+      <c r="D265" s="0" t="n">
+        <v>279.7</v>
+      </c>
+      <c r="E265" s="0" t="n">
+        <v>273.6</v>
+      </c>
+      <c r="F265" s="0" t="n">
+        <v>235</v>
       </c>
       <c r="G265" s="0" t="n">
         <v>3.13</v>
@@ -3714,7 +4755,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G266" s="0" t="n">
         <v>1.88</v>
@@ -3722,7 +4763,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G267" s="0" t="n">
         <v>1.56</v>
@@ -3730,7 +4771,22 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="C268" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="D268" s="0" t="n">
+        <v>355.2</v>
+      </c>
+      <c r="E268" s="0" t="n">
+        <v>470.1</v>
+      </c>
+      <c r="F268" s="0" t="n">
+        <v>525.4</v>
       </c>
       <c r="G268" s="0" t="n">
         <v>2.32</v>
@@ -3738,7 +4794,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G269" s="0" t="n">
         <v>2.58</v>
@@ -3746,7 +4802,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G270" s="0" t="n">
         <v>2.59</v>
@@ -3754,7 +4810,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G271" s="0" t="n">
         <v>2.87</v>
@@ -3762,7 +4818,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G272" s="0" t="n">
         <v>1.86</v>
@@ -3770,7 +4826,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G273" s="0" t="n">
         <v>2.45</v>
@@ -3778,7 +4834,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G274" s="0" t="n">
         <v>1.92</v>
@@ -3786,7 +4842,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G275" s="0" t="n">
         <v>2.68</v>
@@ -3794,7 +4850,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G276" s="0" t="n">
         <v>2.29</v>
@@ -3802,7 +4858,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G277" s="0" t="n">
         <v>1.88</v>
@@ -3810,7 +4866,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G278" s="0" t="n">
         <v>2.17</v>
@@ -3818,7 +4874,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G279" s="0" t="n">
         <v>1.94</v>
@@ -3826,7 +4882,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G280" s="0" t="n">
         <v>2.4</v>
@@ -3834,7 +4890,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G281" s="0" t="n">
         <v>2.22</v>
@@ -3842,7 +4898,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G282" s="0" t="n">
         <v>1.58</v>
@@ -3850,7 +4906,22 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="C283" s="0" t="n">
+        <v>433.8</v>
+      </c>
+      <c r="D283" s="0" t="n">
+        <v>321.7</v>
+      </c>
+      <c r="E283" s="0" t="n">
+        <v>389.6</v>
+      </c>
+      <c r="F283" s="0" t="n">
+        <v>421</v>
       </c>
       <c r="G283" s="0" t="n">
         <v>2.64</v>
@@ -3858,7 +4929,22 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>8.81</v>
+      </c>
+      <c r="C284" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="D284" s="0" t="n">
+        <v>334.9</v>
+      </c>
+      <c r="E284" s="0" t="n">
+        <v>400.5</v>
+      </c>
+      <c r="F284" s="0" t="n">
+        <v>306.4</v>
       </c>
       <c r="G284" s="0" t="n">
         <v>2.14</v>
@@ -3866,7 +4952,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G285" s="0" t="n">
         <v>1.85</v>
@@ -3874,7 +4960,22 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="C286" s="0" t="n">
+        <v>592.7</v>
+      </c>
+      <c r="D286" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="E286" s="0" t="n">
+        <v>413.6</v>
+      </c>
+      <c r="F286" s="0" t="n">
+        <v>447.9</v>
       </c>
       <c r="G286" s="0" t="n">
         <v>3.35</v>
@@ -3882,7 +4983,22 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>8.45</v>
+      </c>
+      <c r="C287" s="0" t="n">
+        <v>369</v>
+      </c>
+      <c r="D287" s="0" t="n">
+        <v>431.1</v>
+      </c>
+      <c r="E287" s="0" t="n">
+        <v>455.6</v>
+      </c>
+      <c r="F287" s="0" t="n">
+        <v>454.9</v>
       </c>
       <c r="G287" s="0" t="n">
         <v>2.09</v>
@@ -3890,7 +5006,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G288" s="0" t="n">
         <v>4.08</v>
@@ -3898,7 +5014,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G289" s="0" t="n">
         <v>2.46</v>
@@ -3906,7 +5022,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G290" s="0" t="n">
         <v>1.74</v>
@@ -3914,7 +5030,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G291" s="0" t="n">
         <v>3.05</v>
@@ -3922,7 +5038,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G292" s="0" t="n">
         <v>2.33</v>
@@ -3930,7 +5046,22 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C293" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="D293" s="0" t="n">
+        <v>264</v>
+      </c>
+      <c r="E293" s="0" t="n">
+        <v>410.7</v>
+      </c>
+      <c r="F293" s="0" t="n">
+        <v>478.6</v>
       </c>
       <c r="G293" s="0" t="n">
         <v>2.42</v>
@@ -3938,7 +5069,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G294" s="0" t="n">
         <v>3.77</v>
@@ -3946,7 +5077,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G295" s="0" t="n">
         <v>3.73</v>
@@ -3954,7 +5085,22 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
+      </c>
+      <c r="B296" s="0" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="C296" s="0" t="n">
+        <v>428</v>
+      </c>
+      <c r="D296" s="0" t="n">
+        <v>301.1</v>
+      </c>
+      <c r="E296" s="0" t="n">
+        <v>381.6</v>
+      </c>
+      <c r="F296" s="0" t="n">
+        <v>375.2</v>
       </c>
       <c r="G296" s="0" t="n">
         <v>2.37</v>
@@ -3962,7 +5108,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G297" s="0" t="n">
         <v>2.89</v>
@@ -3970,7 +5116,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G298" s="0" t="n">
         <v>1.94</v>
@@ -3978,7 +5124,22 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="B299" s="0" t="n">
+        <v>8.16</v>
+      </c>
+      <c r="C299" s="0" t="n">
+        <v>374</v>
+      </c>
+      <c r="D299" s="0" t="n">
+        <v>304.2</v>
+      </c>
+      <c r="E299" s="0" t="n">
+        <v>741.3</v>
+      </c>
+      <c r="F299" s="0" t="n">
+        <v>411.4</v>
       </c>
       <c r="G299" s="0" t="n">
         <v>2.18</v>
@@ -3986,7 +5147,22 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
+      </c>
+      <c r="B300" s="0" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="C300" s="0" t="n">
+        <v>286</v>
+      </c>
+      <c r="D300" s="0" t="n">
+        <v>264</v>
+      </c>
+      <c r="E300" s="0" t="n">
+        <v>330.1</v>
+      </c>
+      <c r="F300" s="0" t="n">
+        <v>321.7</v>
       </c>
       <c r="G300" s="0" t="n">
         <v>1.62</v>
@@ -3994,7 +5170,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G301" s="0" t="n">
         <v>2.56</v>
@@ -4002,7 +5178,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G302" s="0" t="n">
         <v>2.06</v>
@@ -4010,7 +5186,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G303" s="0" t="n">
         <v>2.43</v>
@@ -4018,7 +5194,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G304" s="0" t="n">
         <v>3.02</v>
@@ -4026,7 +5202,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G305" s="0" t="n">
         <v>2.84</v>
@@ -4034,7 +5210,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G306" s="0" t="n">
         <v>1.23</v>
@@ -4042,7 +5218,22 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
+      </c>
+      <c r="B307" s="0" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="C307" s="0" t="n">
+        <v>302.23</v>
+      </c>
+      <c r="D307" s="0" t="n">
+        <v>418</v>
+      </c>
+      <c r="E307" s="0" t="n">
+        <v>463.5</v>
+      </c>
+      <c r="F307" s="0" t="n">
+        <v>434.6</v>
       </c>
       <c r="G307" s="0" t="n">
         <v>1.66</v>
@@ -4050,7 +5241,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B308" s="0" t="n">
         <v>9.28</v>
@@ -4073,7 +5264,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G309" s="0" t="n">
         <v>4.93</v>
@@ -4081,7 +5272,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G310" s="0" t="n">
         <v>2.29</v>
@@ -4089,7 +5280,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G311" s="0" t="n">
         <v>2.73</v>
@@ -4097,7 +5288,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G312" s="0" t="n">
         <v>3.24</v>
@@ -4105,7 +5296,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B313" s="0" t="n">
         <v>14.91</v>
@@ -4128,7 +5319,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G314" s="0" t="n">
         <v>2.25</v>
@@ -4136,7 +5327,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G315" s="0" t="n">
         <v>2.64</v>
@@ -4144,7 +5335,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G316" s="0" t="n">
         <v>2.18</v>
@@ -4152,7 +5343,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G317" s="0" t="n">
         <v>1.58</v>
@@ -4160,7 +5351,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G318" s="0" t="n">
         <v>1.81</v>
@@ -4168,7 +5359,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G319" s="0" t="n">
         <v>3.52</v>
@@ -4176,7 +5367,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G320" s="0" t="n">
         <v>1.98</v>
@@ -4184,7 +5375,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G321" s="0" t="n">
         <v>4.73</v>
@@ -4192,7 +5383,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G322" s="0" t="n">
         <v>3.01</v>
@@ -4200,7 +5391,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G323" s="0" t="n">
         <v>2.82</v>
@@ -4208,7 +5399,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G324" s="0" t="n">
         <v>3.21</v>
@@ -4216,7 +5407,22 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
+      </c>
+      <c r="B325" s="0" t="n">
+        <v>9.54</v>
+      </c>
+      <c r="C325" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="D325" s="0" t="n">
+        <v>265.2</v>
+      </c>
+      <c r="E325" s="0" t="n">
+        <v>278.4</v>
+      </c>
+      <c r="F325" s="0" t="n">
+        <v>315.2</v>
       </c>
       <c r="G325" s="0" t="n">
         <v>2.37</v>
@@ -4224,7 +5430,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G326" s="0" t="n">
         <v>1.82</v>

</xml_diff>